<commit_message>
revising decision models data
</commit_message>
<xml_diff>
--- a/class_materials/data/decision_model.xlsx
+++ b/class_materials/data/decision_model.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Dropbox\Datapolitan\Training\DCAS\github_slides\Data_Analytics_Classes\class_materials\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1680" windowWidth="23920" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="1680" yWindow="1680" windowWidth="23925" windowHeight="15315" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,12 +41,6 @@
     <t>% Collect</t>
   </si>
   <si>
-    <t>Min.</t>
-  </si>
-  <si>
-    <t>Max.</t>
-  </si>
-  <si>
     <t>Manhattan</t>
   </si>
   <si>
@@ -72,17 +71,24 @@
     <t>Agents Assigned</t>
   </si>
   <si>
-    <t>Agents Avaialble</t>
+    <t>Agents Available</t>
+  </si>
+  <si>
+    <t>Minimum Number of Agents Assigned</t>
+  </si>
+  <si>
+    <t>Maximum Number of Agents Assigned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,11 +108,20 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -127,10 +142,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -144,17 +160,27 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -483,15 +509,15 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="60">
+    <row r="1" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,25 +533,25 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="B2" s="5">
         <v>0.4</v>
@@ -546,9 +572,9 @@
         <v>600</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5">
         <v>0.2</v>
@@ -569,9 +595,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5">
         <v>0.15</v>
@@ -592,9 +618,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="5">
         <v>0.1</v>
@@ -615,9 +641,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5">
         <v>0.1</v>
@@ -638,20 +664,21 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G7" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G8" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H9" s="9" t="s">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="I9" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>